<commit_message>
tranfered and plotted 2kod oa we v00 pcs data
</commit_message>
<xml_diff>
--- a/pcs_data/dHis_CTD_PCS_W184.xlsx
+++ b/pcs_data/dHis_CTD_PCS_W184.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darian/Google/MBSB/Research/Projects/hiv1_capsid/calc_pcs_qf/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darian/github/calc_ca_pcs/pcs_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581A99B4-7D3B-ED4C-9840-A0E69EA4ACB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38781CCD-316B-B243-B4E3-3669860EBA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="1" xr2:uid="{F1CAFD48-BBA8-EA44-9E19-F5AFA1BA9D49}"/>
   </bookViews>
@@ -582,7 +582,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.5" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -820,7 +820,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
broke down the inter and intra contributions and noted them for simulated d1 d2 on excel file
</commit_message>
<xml_diff>
--- a/pcs_data/dHis_CTD_PCS_W184.xlsx
+++ b/pcs_data/dHis_CTD_PCS_W184.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darian/github/calc_ca_pcs/pcs_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38781CCD-316B-B243-B4E3-3669860EBA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4D339A-E540-C24B-8EBF-EFA6472D5B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="1" xr2:uid="{F1CAFD48-BBA8-EA44-9E19-F5AFA1BA9D49}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="2" xr2:uid="{F1CAFD48-BBA8-EA44-9E19-F5AFA1BA9D49}"/>
   </bookViews>
   <sheets>
     <sheet name="dHis_CTD_PCS" sheetId="1" r:id="rId1"/>
     <sheet name="Pred_PCS" sheetId="2" r:id="rId2"/>
+    <sheet name="d1d2" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
   <si>
     <t>PDB</t>
   </si>
@@ -140,6 +141,18 @@
   </si>
   <si>
     <t>1a43</t>
+  </si>
+  <si>
+    <t>D1 (Sim)</t>
+  </si>
+  <si>
+    <t>D2 (Sim)</t>
+  </si>
+  <si>
+    <t>intra+inter_HE1</t>
+  </si>
+  <si>
+    <t>intra+inter_HZ2</t>
   </si>
 </sst>
 </file>
@@ -213,7 +226,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -221,11 +234,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -258,6 +311,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -582,7 +662,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.5" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -819,7 +899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE586931-9621-6841-A6FC-87DEAE0D374D}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -1032,4 +1112,305 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122735B3-C6FF-EC4A-A95F-FA229E70C572}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="25.5" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.1640625" style="1" customWidth="1"/>
+    <col min="3" max="6" width="33.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="25.5" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.1482</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.1386</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.17480000000000001</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.1129</v>
+      </c>
+      <c r="F2" s="1">
+        <v>8.1900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>6.3E-2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>5.7799999999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2.7E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>5.21E-2</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="C5" s="3">
+        <v>3.9E-2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="F5" s="1">
+        <v>5.2600000000000001E-2</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="3">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="J5" s="3">
+        <v>7.3999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.105</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6.8900000000000003E-2</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.106</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.13700000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="16" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="14">
+        <f>B3+B4</f>
+        <v>0.108</v>
+      </c>
+      <c r="C7" s="14">
+        <f>C3+C4</f>
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="D7" s="15">
+        <f>D3+D4</f>
+        <v>0.18</v>
+      </c>
+      <c r="E7" s="15">
+        <f t="shared" ref="E7:F7" si="0">E3+E4</f>
+        <v>0.13799999999999998</v>
+      </c>
+      <c r="F7" s="15">
+        <f t="shared" si="0"/>
+        <v>0.1099</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="J7" s="14">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="20" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="18">
+        <f>B5+B6</f>
+        <v>0.153</v>
+      </c>
+      <c r="C8" s="18">
+        <f>C5+C6</f>
+        <v>7.1000000000000008E-2</v>
+      </c>
+      <c r="D8" s="19">
+        <f>D5+D6</f>
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="E8" s="19">
+        <f t="shared" ref="E8:F8" si="1">E5+E6</f>
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="F8" s="19">
+        <f t="shared" si="1"/>
+        <v>0.1215</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="18">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="J8" s="18">
+        <v>0.184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>-3.6850000000000001</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-2.1160000000000001</v>
+      </c>
+      <c r="D10" s="1">
+        <v>-3.3359999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>-0.72299999999999998</v>
+      </c>
+      <c r="C11" s="1">
+        <v>-1.1859999999999999</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-1.444</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>